<commit_message>
Modernize Dashboard UI with Liquid Glass aesthetic and implement user-specific notification system
</commit_message>
<xml_diff>
--- a/data/assets.xlsx
+++ b/data/assets.xlsx
@@ -10,14 +10,14 @@
     <sheet sheetId="1" name="Assets" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase">Assets!$C$1:$M$7</definedName>
+    <definedName name="_xlnm._FilterDatabase">Assets!$C$1:$M$3</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -91,6 +91,33 @@
     <t>passId</t>
   </si>
   <si>
+    <t>transfer_status</t>
+  </si>
+  <si>
+    <t>rejection_reason</t>
+  </si>
+  <si>
+    <t>rejected_by</t>
+  </si>
+  <si>
+    <t>rejected_at</t>
+  </si>
+  <si>
+    <t>gate_pass_type</t>
+  </si>
+  <si>
+    <t>amc_warranty</t>
+  </si>
+  <si>
+    <t>branch_user</t>
+  </si>
+  <si>
+    <t>from_branch</t>
+  </si>
+  <si>
+    <t>from_branch_code</t>
+  </si>
+  <si>
     <t>Workstation</t>
   </si>
   <si>
@@ -109,88 +136,133 @@
     <t>Admin</t>
   </si>
   <si>
+    <t>Disposed</t>
+  </si>
+  <si>
+    <t>2026-01-26T16:41:23.258Z</t>
+  </si>
+  <si>
+    <t>Damaged</t>
+  </si>
+  <si>
+    <t>Admin ID</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:36:55.453Z</t>
+  </si>
+  <si>
+    <t>HP ProDesk</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>TransferInitiated</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Thanjaur</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Test Asset</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>2022-01-04</t>
+  </si>
+  <si>
+    <t>2026-01-29</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>54321</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:33:53.325Z</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:34:13.140Z</t>
+  </si>
+  <si>
+    <t>test asset1_TR_1769715215790</t>
+  </si>
+  <si>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>2028-01-03</t>
+  </si>
+  <si>
+    <t>123463</t>
+  </si>
+  <si>
+    <t>Transferred</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:31:26.371Z</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:33:35.697Z</t>
+  </si>
+  <si>
+    <t>test asset1_TR_1769715326810</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:35:21.227Z</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>2026-01-29T19:35:26.744Z</t>
+  </si>
+  <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>New Asset</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Asset2</t>
+  </si>
+  <si>
+    <t>2026-01-02</t>
+  </si>
+  <si>
+    <t>2027-01-01</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>DisposalInitiated</t>
-  </si>
-  <si>
-    <t>2026-01-26T16:41:23.258Z</t>
-  </si>
-  <si>
-    <t>Damaged</t>
-  </si>
-  <si>
-    <t>Initiated</t>
-  </si>
-  <si>
-    <t>HP ProDesk</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Warranty</t>
-  </si>
-  <si>
-    <t>Projector</t>
-  </si>
-  <si>
-    <t>12959</t>
-  </si>
-  <si>
-    <t>2021-02-19T00:00:00.000Z</t>
-  </si>
-  <si>
-    <t>2022-02-27T00:00:00.000Z</t>
-  </si>
-  <si>
-    <t>123463</t>
-  </si>
-  <si>
-    <t>GatePass</t>
-  </si>
-  <si>
-    <t>Auditoruim</t>
-  </si>
-  <si>
-    <t>Presentation</t>
-  </si>
-  <si>
-    <t>Use</t>
-  </si>
-  <si>
-    <t>Pass0001</t>
-  </si>
-  <si>
-    <t>TransferInitiated</t>
-  </si>
-  <si>
-    <t>Transfer</t>
-  </si>
-  <si>
-    <t>Thanjaur</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>ApprovalPending</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>2026-01-09</t>
-  </si>
-  <si>
-    <t>Manager2</t>
-  </si>
-  <si>
-    <t>TransferApprovalPending</t>
+    <t>2026-01-29T20:07:34.371Z</t>
+  </si>
+  <si>
+    <t>new employee</t>
+  </si>
+  <si>
+    <t>2026-01-29T20:07:40.012Z</t>
   </si>
 </sst>
 </file>
@@ -573,7 +645,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA260"/>
+  <dimension ref="A1:AG259"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="N9" sqref="N9"/>
@@ -595,482 +667,332 @@
     <col min="14" max="14" width="9.05078125" customWidth="1"/>
     <col min="15" max="15" width="8.83984375" customWidth="1"/>
     <col min="16" max="16" width="6.05078125" customWidth="1"/>
-    <col min="17" max="17" width="5.3671875" customWidth="1"/>
-    <col min="18" max="18" width="10.15625" customWidth="1"/>
-    <col min="19" max="19" width="9.9453125" customWidth="1"/>
+    <col min="17" max="17" width="10.15625" customWidth="1"/>
+    <col min="18" max="18" width="9.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>841</v>
+        <v>957</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1">
-        <v>12841</v>
+        <v>12957</v>
       </c>
       <c r="F2" s="2">
-        <v>44628</v>
+        <v>42535</v>
       </c>
       <c r="G2" s="2">
         <v>44619</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1">
         <v>123463</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1">
-        <v>12957</v>
+        <v>12960</v>
       </c>
       <c r="F3" s="2">
-        <v>42535</v>
+        <v>42704</v>
       </c>
       <c r="G3" s="2">
-        <v>44619</v>
+        <v>44529</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1">
         <v>123463</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>958</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3">
+        <v>123463</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="1">
-        <v>12958</v>
-      </c>
-      <c r="F4" s="2">
-        <v>42794</v>
-      </c>
-      <c r="G4" s="2">
-        <v>46445</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="1">
-        <v>123463</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="X3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>959</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="5" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5" s="1">
-        <v>123463</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>960</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="1">
-        <v>12960</v>
-      </c>
-      <c r="F6" s="2">
-        <v>42704</v>
-      </c>
-      <c r="G6" s="2">
-        <v>44529</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="1">
-        <v>123463</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>48</v>
-      </c>
+    </row>
+    <row r="6" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V6" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X6">
-        <v>123463</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1211</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1">
-        <v>12961</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="2">
-        <v>44619</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="1">
-        <v>54320</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="7" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-    </row>
-    <row r="8" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>960</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12960</v>
-      </c>
-      <c r="F8" s="2">
-        <v>42704</v>
-      </c>
-      <c r="G8" s="2">
-        <v>44529</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="1">
-        <v>54320</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>57</v>
-      </c>
+    </row>
+    <row r="8" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1089,9 +1011,8 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1110,9 +1031,8 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-    </row>
-    <row r="11" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1131,9 +1051,8 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-    </row>
-    <row r="12" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1152,9 +1071,8 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-    </row>
-    <row r="13" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1173,9 +1091,8 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-    </row>
-    <row r="14" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1194,9 +1111,8 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-    </row>
-    <row r="15" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1215,9 +1131,8 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-    </row>
-    <row r="16" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1236,9 +1151,8 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1257,9 +1171,8 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-    </row>
-    <row r="18" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1278,9 +1191,8 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-    </row>
-    <row r="19" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1299,9 +1211,8 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1320,9 +1231,8 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-    </row>
-    <row r="21" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1341,9 +1251,8 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1362,9 +1271,8 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1383,9 +1291,8 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1404,9 +1311,8 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1425,9 +1331,8 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1446,9 +1351,8 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-    </row>
-    <row r="27" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1467,9 +1371,8 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-    </row>
-    <row r="28" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1488,9 +1391,8 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1509,9 +1411,8 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1530,9 +1431,8 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-    </row>
-    <row r="31" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1551,9 +1451,8 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1572,9 +1471,8 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-    </row>
-    <row r="33" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1593,9 +1491,8 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-    </row>
-    <row r="34" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1614,9 +1511,8 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-    </row>
-    <row r="35" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1635,9 +1531,8 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1656,9 +1551,8 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1677,9 +1571,8 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-    </row>
-    <row r="38" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1698,9 +1591,8 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-    </row>
-    <row r="39" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1719,9 +1611,8 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-    </row>
-    <row r="40" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1740,9 +1631,8 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1761,9 +1651,8 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-    </row>
-    <row r="42" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1782,9 +1671,8 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-    </row>
-    <row r="43" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1803,9 +1691,8 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-    </row>
-    <row r="44" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1824,9 +1711,8 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-    </row>
-    <row r="45" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1845,9 +1731,8 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-    </row>
-    <row r="46" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1866,9 +1751,8 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-    </row>
-    <row r="47" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1887,9 +1771,8 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-    </row>
-    <row r="48" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1908,9 +1791,8 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-    </row>
-    <row r="49" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1929,9 +1811,8 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-    </row>
-    <row r="50" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1950,9 +1831,8 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-    </row>
-    <row r="51" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1971,9 +1851,8 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-    </row>
-    <row r="52" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1992,9 +1871,8 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-    </row>
-    <row r="53" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2013,9 +1891,8 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-    </row>
-    <row r="54" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2034,9 +1911,8 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-    </row>
-    <row r="55" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2055,9 +1931,8 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-    </row>
-    <row r="56" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2076,9 +1951,8 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-    </row>
-    <row r="57" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2097,9 +1971,8 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-    </row>
-    <row r="58" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2118,9 +1991,8 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-    </row>
-    <row r="59" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2139,9 +2011,8 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-    </row>
-    <row r="60" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2160,9 +2031,8 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-    </row>
-    <row r="61" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2181,9 +2051,8 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-    </row>
-    <row r="62" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2202,9 +2071,8 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-    </row>
-    <row r="63" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2223,9 +2091,8 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-    </row>
-    <row r="64" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2244,9 +2111,8 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-    </row>
-    <row r="65" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2265,9 +2131,8 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-    </row>
-    <row r="66" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2286,9 +2151,8 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-    </row>
-    <row r="67" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2307,9 +2171,8 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-    </row>
-    <row r="68" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2328,9 +2191,8 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-    </row>
-    <row r="69" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2349,9 +2211,8 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-    </row>
-    <row r="70" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2370,9 +2231,8 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-    </row>
-    <row r="71" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2391,9 +2251,8 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-    </row>
-    <row r="72" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2412,9 +2271,8 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-    </row>
-    <row r="73" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2433,9 +2291,8 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-    </row>
-    <row r="74" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2454,9 +2311,8 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-    </row>
-    <row r="75" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2475,9 +2331,8 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-    </row>
-    <row r="76" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2496,9 +2351,8 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
-      <c r="S76" s="1"/>
-    </row>
-    <row r="77" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2517,9 +2371,8 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-    </row>
-    <row r="78" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2538,9 +2391,8 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-    </row>
-    <row r="79" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2559,9 +2411,8 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
-    </row>
-    <row r="80" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2580,9 +2431,8 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-    </row>
-    <row r="81" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2601,9 +2451,8 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
-      <c r="S81" s="1"/>
-    </row>
-    <row r="82" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2622,9 +2471,8 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
-      <c r="S82" s="1"/>
-    </row>
-    <row r="83" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2643,9 +2491,8 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
-    </row>
-    <row r="84" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2664,9 +2511,8 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
-      <c r="S84" s="1"/>
-    </row>
-    <row r="85" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2685,9 +2531,8 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
-      <c r="S85" s="1"/>
-    </row>
-    <row r="86" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2706,9 +2551,8 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
-    </row>
-    <row r="87" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2727,9 +2571,8 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
-      <c r="S87" s="1"/>
-    </row>
-    <row r="88" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2748,9 +2591,8 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
-      <c r="S88" s="1"/>
-    </row>
-    <row r="89" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2769,9 +2611,8 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
-      <c r="S89" s="1"/>
-    </row>
-    <row r="90" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2790,9 +2631,8 @@
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
-      <c r="S90" s="1"/>
-    </row>
-    <row r="91" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2811,9 +2651,8 @@
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
-      <c r="S91" s="1"/>
-    </row>
-    <row r="92" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2832,9 +2671,8 @@
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
-      <c r="S92" s="1"/>
-    </row>
-    <row r="93" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2853,9 +2691,8 @@
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
-      <c r="S93" s="1"/>
-    </row>
-    <row r="94" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2874,9 +2711,8 @@
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
-      <c r="S94" s="1"/>
-    </row>
-    <row r="95" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2895,9 +2731,8 @@
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
-      <c r="S95" s="1"/>
-    </row>
-    <row r="96" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2916,9 +2751,8 @@
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
-      <c r="S96" s="1"/>
-    </row>
-    <row r="97" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2937,9 +2771,8 @@
       <c r="P97" s="1"/>
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
-      <c r="S97" s="1"/>
-    </row>
-    <row r="98" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2958,9 +2791,8 @@
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
-      <c r="S98" s="1"/>
-    </row>
-    <row r="99" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2979,9 +2811,8 @@
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
-      <c r="S99" s="1"/>
-    </row>
-    <row r="100" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3000,9 +2831,8 @@
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-    </row>
-    <row r="101" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3021,9 +2851,8 @@
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
-      <c r="S101" s="1"/>
-    </row>
-    <row r="102" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3042,9 +2871,8 @@
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-    </row>
-    <row r="103" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3063,9 +2891,8 @@
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-    </row>
-    <row r="104" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3084,9 +2911,8 @@
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
-      <c r="S104" s="1"/>
-    </row>
-    <row r="105" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3105,9 +2931,8 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
-      <c r="S105" s="1"/>
-    </row>
-    <row r="106" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3126,9 +2951,8 @@
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
-      <c r="S106" s="1"/>
-    </row>
-    <row r="107" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3147,9 +2971,8 @@
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
-      <c r="S107" s="1"/>
-    </row>
-    <row r="108" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3168,9 +2991,8 @@
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
-      <c r="S108" s="1"/>
-    </row>
-    <row r="109" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3189,9 +3011,8 @@
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
-      <c r="S109" s="1"/>
-    </row>
-    <row r="110" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3210,9 +3031,8 @@
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
-      <c r="S110" s="1"/>
-    </row>
-    <row r="111" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3231,9 +3051,8 @@
       <c r="P111" s="1"/>
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
-      <c r="S111" s="1"/>
-    </row>
-    <row r="112" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3252,9 +3071,8 @@
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
-      <c r="S112" s="1"/>
-    </row>
-    <row r="113" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3273,9 +3091,8 @@
       <c r="P113" s="1"/>
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
-      <c r="S113" s="1"/>
-    </row>
-    <row r="114" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3294,9 +3111,8 @@
       <c r="P114" s="1"/>
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
-      <c r="S114" s="1"/>
-    </row>
-    <row r="115" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3315,9 +3131,8 @@
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
-      <c r="S115" s="1"/>
-    </row>
-    <row r="116" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3336,9 +3151,8 @@
       <c r="P116" s="1"/>
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
-      <c r="S116" s="1"/>
-    </row>
-    <row r="117" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3357,9 +3171,8 @@
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
-      <c r="S117" s="1"/>
-    </row>
-    <row r="118" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3378,9 +3191,8 @@
       <c r="P118" s="1"/>
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
-      <c r="S118" s="1"/>
-    </row>
-    <row r="119" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3399,9 +3211,8 @@
       <c r="P119" s="1"/>
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
-      <c r="S119" s="1"/>
-    </row>
-    <row r="120" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3420,9 +3231,8 @@
       <c r="P120" s="1"/>
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
-      <c r="S120" s="1"/>
-    </row>
-    <row r="121" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3441,9 +3251,8 @@
       <c r="P121" s="1"/>
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
-      <c r="S121" s="1"/>
-    </row>
-    <row r="122" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3462,9 +3271,8 @@
       <c r="P122" s="1"/>
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
-      <c r="S122" s="1"/>
-    </row>
-    <row r="123" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3483,9 +3291,8 @@
       <c r="P123" s="1"/>
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
-      <c r="S123" s="1"/>
-    </row>
-    <row r="124" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3504,9 +3311,8 @@
       <c r="P124" s="1"/>
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
-      <c r="S124" s="1"/>
-    </row>
-    <row r="125" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3525,9 +3331,8 @@
       <c r="P125" s="1"/>
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
-      <c r="S125" s="1"/>
-    </row>
-    <row r="126" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3546,9 +3351,8 @@
       <c r="P126" s="1"/>
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
-      <c r="S126" s="1"/>
-    </row>
-    <row r="127" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3567,9 +3371,8 @@
       <c r="P127" s="1"/>
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
-      <c r="S127" s="1"/>
-    </row>
-    <row r="128" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3588,9 +3391,8 @@
       <c r="P128" s="1"/>
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
-      <c r="S128" s="1"/>
-    </row>
-    <row r="129" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3609,9 +3411,8 @@
       <c r="P129" s="1"/>
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
-      <c r="S129" s="1"/>
-    </row>
-    <row r="130" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3630,9 +3431,8 @@
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
-      <c r="S130" s="1"/>
-    </row>
-    <row r="131" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3651,9 +3451,8 @@
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
-      <c r="S131" s="1"/>
-    </row>
-    <row r="132" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3672,9 +3471,8 @@
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
-      <c r="S132" s="1"/>
-    </row>
-    <row r="133" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3693,9 +3491,8 @@
       <c r="P133" s="1"/>
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
-      <c r="S133" s="1"/>
-    </row>
-    <row r="134" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3714,9 +3511,8 @@
       <c r="P134" s="1"/>
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
-      <c r="S134" s="1"/>
-    </row>
-    <row r="135" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3735,9 +3531,8 @@
       <c r="P135" s="1"/>
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
-      <c r="S135" s="1"/>
-    </row>
-    <row r="136" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3756,9 +3551,8 @@
       <c r="P136" s="1"/>
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
-      <c r="S136" s="1"/>
-    </row>
-    <row r="137" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3777,9 +3571,8 @@
       <c r="P137" s="1"/>
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
-      <c r="S137" s="1"/>
-    </row>
-    <row r="138" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3798,9 +3591,8 @@
       <c r="P138" s="1"/>
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
-      <c r="S138" s="1"/>
-    </row>
-    <row r="139" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3819,9 +3611,8 @@
       <c r="P139" s="1"/>
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
-      <c r="S139" s="1"/>
-    </row>
-    <row r="140" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3840,9 +3631,8 @@
       <c r="P140" s="1"/>
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
-      <c r="S140" s="1"/>
-    </row>
-    <row r="141" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3861,9 +3651,8 @@
       <c r="P141" s="1"/>
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
-      <c r="S141" s="1"/>
-    </row>
-    <row r="142" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3882,9 +3671,8 @@
       <c r="P142" s="1"/>
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
-      <c r="S142" s="1"/>
-    </row>
-    <row r="143" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3903,9 +3691,8 @@
       <c r="P143" s="1"/>
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
-      <c r="S143" s="1"/>
-    </row>
-    <row r="144" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3924,9 +3711,8 @@
       <c r="P144" s="1"/>
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
-      <c r="S144" s="1"/>
-    </row>
-    <row r="145" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3945,9 +3731,8 @@
       <c r="P145" s="1"/>
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
-      <c r="S145" s="1"/>
-    </row>
-    <row r="146" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3966,9 +3751,8 @@
       <c r="P146" s="1"/>
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
-      <c r="S146" s="1"/>
-    </row>
-    <row r="147" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3987,9 +3771,8 @@
       <c r="P147" s="1"/>
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
-      <c r="S147" s="1"/>
-    </row>
-    <row r="148" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4008,9 +3791,8 @@
       <c r="P148" s="1"/>
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
-      <c r="S148" s="1"/>
-    </row>
-    <row r="149" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4029,9 +3811,8 @@
       <c r="P149" s="1"/>
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
-      <c r="S149" s="1"/>
-    </row>
-    <row r="150" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4050,9 +3831,8 @@
       <c r="P150" s="1"/>
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
-      <c r="S150" s="1"/>
-    </row>
-    <row r="151" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4071,9 +3851,8 @@
       <c r="P151" s="1"/>
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
-      <c r="S151" s="1"/>
-    </row>
-    <row r="152" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4092,9 +3871,8 @@
       <c r="P152" s="1"/>
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
-      <c r="S152" s="1"/>
-    </row>
-    <row r="153" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4113,9 +3891,8 @@
       <c r="P153" s="1"/>
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
-      <c r="S153" s="1"/>
-    </row>
-    <row r="154" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4134,9 +3911,8 @@
       <c r="P154" s="1"/>
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
-      <c r="S154" s="1"/>
-    </row>
-    <row r="155" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4155,9 +3931,8 @@
       <c r="P155" s="1"/>
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
-      <c r="S155" s="1"/>
-    </row>
-    <row r="156" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4176,9 +3951,8 @@
       <c r="P156" s="1"/>
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
-      <c r="S156" s="1"/>
-    </row>
-    <row r="157" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4197,9 +3971,8 @@
       <c r="P157" s="1"/>
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
-      <c r="S157" s="1"/>
-    </row>
-    <row r="158" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4218,9 +3991,8 @@
       <c r="P158" s="1"/>
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
-      <c r="S158" s="1"/>
-    </row>
-    <row r="159" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4239,9 +4011,8 @@
       <c r="P159" s="1"/>
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
-      <c r="S159" s="1"/>
-    </row>
-    <row r="160" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4260,9 +4031,8 @@
       <c r="P160" s="1"/>
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
-      <c r="S160" s="1"/>
-    </row>
-    <row r="161" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4281,9 +4051,8 @@
       <c r="P161" s="1"/>
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
-      <c r="S161" s="1"/>
-    </row>
-    <row r="162" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4302,9 +4071,8 @@
       <c r="P162" s="1"/>
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
-      <c r="S162" s="1"/>
-    </row>
-    <row r="163" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4323,9 +4091,8 @@
       <c r="P163" s="1"/>
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
-      <c r="S163" s="1"/>
-    </row>
-    <row r="164" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4344,9 +4111,8 @@
       <c r="P164" s="1"/>
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
-      <c r="S164" s="1"/>
-    </row>
-    <row r="165" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4365,9 +4131,8 @@
       <c r="P165" s="1"/>
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
-      <c r="S165" s="1"/>
-    </row>
-    <row r="166" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4386,9 +4151,8 @@
       <c r="P166" s="1"/>
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
-      <c r="S166" s="1"/>
-    </row>
-    <row r="167" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4407,9 +4171,8 @@
       <c r="P167" s="1"/>
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
-      <c r="S167" s="1"/>
-    </row>
-    <row r="168" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4428,9 +4191,8 @@
       <c r="P168" s="1"/>
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
-      <c r="S168" s="1"/>
-    </row>
-    <row r="169" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4449,9 +4211,8 @@
       <c r="P169" s="1"/>
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
-      <c r="S169" s="1"/>
-    </row>
-    <row r="170" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4470,9 +4231,8 @@
       <c r="P170" s="1"/>
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
-      <c r="S170" s="1"/>
-    </row>
-    <row r="171" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4491,9 +4251,8 @@
       <c r="P171" s="1"/>
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
-      <c r="S171" s="1"/>
-    </row>
-    <row r="172" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4512,9 +4271,8 @@
       <c r="P172" s="1"/>
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
-      <c r="S172" s="1"/>
-    </row>
-    <row r="173" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4533,9 +4291,8 @@
       <c r="P173" s="1"/>
       <c r="Q173" s="1"/>
       <c r="R173" s="1"/>
-      <c r="S173" s="1"/>
-    </row>
-    <row r="174" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4554,9 +4311,8 @@
       <c r="P174" s="1"/>
       <c r="Q174" s="1"/>
       <c r="R174" s="1"/>
-      <c r="S174" s="1"/>
-    </row>
-    <row r="175" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4575,9 +4331,8 @@
       <c r="P175" s="1"/>
       <c r="Q175" s="1"/>
       <c r="R175" s="1"/>
-      <c r="S175" s="1"/>
-    </row>
-    <row r="176" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4596,9 +4351,8 @@
       <c r="P176" s="1"/>
       <c r="Q176" s="1"/>
       <c r="R176" s="1"/>
-      <c r="S176" s="1"/>
-    </row>
-    <row r="177" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4617,9 +4371,8 @@
       <c r="P177" s="1"/>
       <c r="Q177" s="1"/>
       <c r="R177" s="1"/>
-      <c r="S177" s="1"/>
-    </row>
-    <row r="178" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4638,9 +4391,8 @@
       <c r="P178" s="1"/>
       <c r="Q178" s="1"/>
       <c r="R178" s="1"/>
-      <c r="S178" s="1"/>
-    </row>
-    <row r="179" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4659,9 +4411,8 @@
       <c r="P179" s="1"/>
       <c r="Q179" s="1"/>
       <c r="R179" s="1"/>
-      <c r="S179" s="1"/>
-    </row>
-    <row r="180" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4680,9 +4431,8 @@
       <c r="P180" s="1"/>
       <c r="Q180" s="1"/>
       <c r="R180" s="1"/>
-      <c r="S180" s="1"/>
-    </row>
-    <row r="181" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4701,9 +4451,8 @@
       <c r="P181" s="1"/>
       <c r="Q181" s="1"/>
       <c r="R181" s="1"/>
-      <c r="S181" s="1"/>
-    </row>
-    <row r="182" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4722,9 +4471,8 @@
       <c r="P182" s="1"/>
       <c r="Q182" s="1"/>
       <c r="R182" s="1"/>
-      <c r="S182" s="1"/>
-    </row>
-    <row r="183" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4743,9 +4491,8 @@
       <c r="P183" s="1"/>
       <c r="Q183" s="1"/>
       <c r="R183" s="1"/>
-      <c r="S183" s="1"/>
-    </row>
-    <row r="184" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4764,9 +4511,8 @@
       <c r="P184" s="1"/>
       <c r="Q184" s="1"/>
       <c r="R184" s="1"/>
-      <c r="S184" s="1"/>
-    </row>
-    <row r="185" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4785,9 +4531,8 @@
       <c r="P185" s="1"/>
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
-      <c r="S185" s="1"/>
-    </row>
-    <row r="186" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4806,9 +4551,8 @@
       <c r="P186" s="1"/>
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
-      <c r="S186" s="1"/>
-    </row>
-    <row r="187" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4827,9 +4571,8 @@
       <c r="P187" s="1"/>
       <c r="Q187" s="1"/>
       <c r="R187" s="1"/>
-      <c r="S187" s="1"/>
-    </row>
-    <row r="188" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4848,9 +4591,8 @@
       <c r="P188" s="1"/>
       <c r="Q188" s="1"/>
       <c r="R188" s="1"/>
-      <c r="S188" s="1"/>
-    </row>
-    <row r="189" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4869,9 +4611,8 @@
       <c r="P189" s="1"/>
       <c r="Q189" s="1"/>
       <c r="R189" s="1"/>
-      <c r="S189" s="1"/>
-    </row>
-    <row r="190" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4890,9 +4631,8 @@
       <c r="P190" s="1"/>
       <c r="Q190" s="1"/>
       <c r="R190" s="1"/>
-      <c r="S190" s="1"/>
-    </row>
-    <row r="191" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4911,9 +4651,8 @@
       <c r="P191" s="1"/>
       <c r="Q191" s="1"/>
       <c r="R191" s="1"/>
-      <c r="S191" s="1"/>
-    </row>
-    <row r="192" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4932,9 +4671,8 @@
       <c r="P192" s="1"/>
       <c r="Q192" s="1"/>
       <c r="R192" s="1"/>
-      <c r="S192" s="1"/>
-    </row>
-    <row r="193" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4953,9 +4691,8 @@
       <c r="P193" s="1"/>
       <c r="Q193" s="1"/>
       <c r="R193" s="1"/>
-      <c r="S193" s="1"/>
-    </row>
-    <row r="194" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4974,9 +4711,8 @@
       <c r="P194" s="1"/>
       <c r="Q194" s="1"/>
       <c r="R194" s="1"/>
-      <c r="S194" s="1"/>
-    </row>
-    <row r="195" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4995,9 +4731,8 @@
       <c r="P195" s="1"/>
       <c r="Q195" s="1"/>
       <c r="R195" s="1"/>
-      <c r="S195" s="1"/>
-    </row>
-    <row r="196" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -5016,9 +4751,8 @@
       <c r="P196" s="1"/>
       <c r="Q196" s="1"/>
       <c r="R196" s="1"/>
-      <c r="S196" s="1"/>
-    </row>
-    <row r="197" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -5037,9 +4771,8 @@
       <c r="P197" s="1"/>
       <c r="Q197" s="1"/>
       <c r="R197" s="1"/>
-      <c r="S197" s="1"/>
-    </row>
-    <row r="198" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -5058,9 +4791,8 @@
       <c r="P198" s="1"/>
       <c r="Q198" s="1"/>
       <c r="R198" s="1"/>
-      <c r="S198" s="1"/>
-    </row>
-    <row r="199" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -5079,9 +4811,8 @@
       <c r="P199" s="1"/>
       <c r="Q199" s="1"/>
       <c r="R199" s="1"/>
-      <c r="S199" s="1"/>
-    </row>
-    <row r="200" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -5100,9 +4831,8 @@
       <c r="P200" s="1"/>
       <c r="Q200" s="1"/>
       <c r="R200" s="1"/>
-      <c r="S200" s="1"/>
-    </row>
-    <row r="201" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -5121,9 +4851,8 @@
       <c r="P201" s="1"/>
       <c r="Q201" s="1"/>
       <c r="R201" s="1"/>
-      <c r="S201" s="1"/>
-    </row>
-    <row r="202" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -5142,9 +4871,8 @@
       <c r="P202" s="1"/>
       <c r="Q202" s="1"/>
       <c r="R202" s="1"/>
-      <c r="S202" s="1"/>
-    </row>
-    <row r="203" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -5163,9 +4891,8 @@
       <c r="P203" s="1"/>
       <c r="Q203" s="1"/>
       <c r="R203" s="1"/>
-      <c r="S203" s="1"/>
-    </row>
-    <row r="204" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -5184,9 +4911,8 @@
       <c r="P204" s="1"/>
       <c r="Q204" s="1"/>
       <c r="R204" s="1"/>
-      <c r="S204" s="1"/>
-    </row>
-    <row r="205" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -5205,9 +4931,8 @@
       <c r="P205" s="1"/>
       <c r="Q205" s="1"/>
       <c r="R205" s="1"/>
-      <c r="S205" s="1"/>
-    </row>
-    <row r="206" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -5226,9 +4951,8 @@
       <c r="P206" s="1"/>
       <c r="Q206" s="1"/>
       <c r="R206" s="1"/>
-      <c r="S206" s="1"/>
-    </row>
-    <row r="207" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -5247,9 +4971,8 @@
       <c r="P207" s="1"/>
       <c r="Q207" s="1"/>
       <c r="R207" s="1"/>
-      <c r="S207" s="1"/>
-    </row>
-    <row r="208" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -5268,9 +4991,8 @@
       <c r="P208" s="1"/>
       <c r="Q208" s="1"/>
       <c r="R208" s="1"/>
-      <c r="S208" s="1"/>
-    </row>
-    <row r="209" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -5289,9 +5011,8 @@
       <c r="P209" s="1"/>
       <c r="Q209" s="1"/>
       <c r="R209" s="1"/>
-      <c r="S209" s="1"/>
-    </row>
-    <row r="210" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -5310,9 +5031,8 @@
       <c r="P210" s="1"/>
       <c r="Q210" s="1"/>
       <c r="R210" s="1"/>
-      <c r="S210" s="1"/>
-    </row>
-    <row r="211" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -5331,9 +5051,8 @@
       <c r="P211" s="1"/>
       <c r="Q211" s="1"/>
       <c r="R211" s="1"/>
-      <c r="S211" s="1"/>
-    </row>
-    <row r="212" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -5352,9 +5071,8 @@
       <c r="P212" s="1"/>
       <c r="Q212" s="1"/>
       <c r="R212" s="1"/>
-      <c r="S212" s="1"/>
-    </row>
-    <row r="213" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -5373,9 +5091,8 @@
       <c r="P213" s="1"/>
       <c r="Q213" s="1"/>
       <c r="R213" s="1"/>
-      <c r="S213" s="1"/>
-    </row>
-    <row r="214" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -5394,9 +5111,8 @@
       <c r="P214" s="1"/>
       <c r="Q214" s="1"/>
       <c r="R214" s="1"/>
-      <c r="S214" s="1"/>
-    </row>
-    <row r="215" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -5415,9 +5131,8 @@
       <c r="P215" s="1"/>
       <c r="Q215" s="1"/>
       <c r="R215" s="1"/>
-      <c r="S215" s="1"/>
-    </row>
-    <row r="216" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -5436,9 +5151,8 @@
       <c r="P216" s="1"/>
       <c r="Q216" s="1"/>
       <c r="R216" s="1"/>
-      <c r="S216" s="1"/>
-    </row>
-    <row r="217" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -5457,9 +5171,8 @@
       <c r="P217" s="1"/>
       <c r="Q217" s="1"/>
       <c r="R217" s="1"/>
-      <c r="S217" s="1"/>
-    </row>
-    <row r="218" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -5478,9 +5191,8 @@
       <c r="P218" s="1"/>
       <c r="Q218" s="1"/>
       <c r="R218" s="1"/>
-      <c r="S218" s="1"/>
-    </row>
-    <row r="219" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -5499,9 +5211,8 @@
       <c r="P219" s="1"/>
       <c r="Q219" s="1"/>
       <c r="R219" s="1"/>
-      <c r="S219" s="1"/>
-    </row>
-    <row r="220" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -5520,9 +5231,8 @@
       <c r="P220" s="1"/>
       <c r="Q220" s="1"/>
       <c r="R220" s="1"/>
-      <c r="S220" s="1"/>
-    </row>
-    <row r="221" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -5541,9 +5251,8 @@
       <c r="P221" s="1"/>
       <c r="Q221" s="1"/>
       <c r="R221" s="1"/>
-      <c r="S221" s="1"/>
-    </row>
-    <row r="222" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -5562,9 +5271,8 @@
       <c r="P222" s="1"/>
       <c r="Q222" s="1"/>
       <c r="R222" s="1"/>
-      <c r="S222" s="1"/>
-    </row>
-    <row r="223" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -5583,9 +5291,8 @@
       <c r="P223" s="1"/>
       <c r="Q223" s="1"/>
       <c r="R223" s="1"/>
-      <c r="S223" s="1"/>
-    </row>
-    <row r="224" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -5604,9 +5311,8 @@
       <c r="P224" s="1"/>
       <c r="Q224" s="1"/>
       <c r="R224" s="1"/>
-      <c r="S224" s="1"/>
-    </row>
-    <row r="225" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -5625,9 +5331,8 @@
       <c r="P225" s="1"/>
       <c r="Q225" s="1"/>
       <c r="R225" s="1"/>
-      <c r="S225" s="1"/>
-    </row>
-    <row r="226" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -5646,9 +5351,8 @@
       <c r="P226" s="1"/>
       <c r="Q226" s="1"/>
       <c r="R226" s="1"/>
-      <c r="S226" s="1"/>
-    </row>
-    <row r="227" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -5667,9 +5371,8 @@
       <c r="P227" s="1"/>
       <c r="Q227" s="1"/>
       <c r="R227" s="1"/>
-      <c r="S227" s="1"/>
-    </row>
-    <row r="228" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -5688,9 +5391,8 @@
       <c r="P228" s="1"/>
       <c r="Q228" s="1"/>
       <c r="R228" s="1"/>
-      <c r="S228" s="1"/>
-    </row>
-    <row r="229" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -5709,9 +5411,8 @@
       <c r="P229" s="1"/>
       <c r="Q229" s="1"/>
       <c r="R229" s="1"/>
-      <c r="S229" s="1"/>
-    </row>
-    <row r="230" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -5730,9 +5431,8 @@
       <c r="P230" s="1"/>
       <c r="Q230" s="1"/>
       <c r="R230" s="1"/>
-      <c r="S230" s="1"/>
-    </row>
-    <row r="231" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -5751,9 +5451,8 @@
       <c r="P231" s="1"/>
       <c r="Q231" s="1"/>
       <c r="R231" s="1"/>
-      <c r="S231" s="1"/>
-    </row>
-    <row r="232" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -5772,9 +5471,8 @@
       <c r="P232" s="1"/>
       <c r="Q232" s="1"/>
       <c r="R232" s="1"/>
-      <c r="S232" s="1"/>
-    </row>
-    <row r="233" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -5793,9 +5491,8 @@
       <c r="P233" s="1"/>
       <c r="Q233" s="1"/>
       <c r="R233" s="1"/>
-      <c r="S233" s="1"/>
-    </row>
-    <row r="234" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -5814,9 +5511,8 @@
       <c r="P234" s="1"/>
       <c r="Q234" s="1"/>
       <c r="R234" s="1"/>
-      <c r="S234" s="1"/>
-    </row>
-    <row r="235" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -5835,9 +5531,8 @@
       <c r="P235" s="1"/>
       <c r="Q235" s="1"/>
       <c r="R235" s="1"/>
-      <c r="S235" s="1"/>
-    </row>
-    <row r="236" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -5856,9 +5551,8 @@
       <c r="P236" s="1"/>
       <c r="Q236" s="1"/>
       <c r="R236" s="1"/>
-      <c r="S236" s="1"/>
-    </row>
-    <row r="237" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -5877,9 +5571,8 @@
       <c r="P237" s="1"/>
       <c r="Q237" s="1"/>
       <c r="R237" s="1"/>
-      <c r="S237" s="1"/>
-    </row>
-    <row r="238" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -5898,9 +5591,8 @@
       <c r="P238" s="1"/>
       <c r="Q238" s="1"/>
       <c r="R238" s="1"/>
-      <c r="S238" s="1"/>
-    </row>
-    <row r="239" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -5919,9 +5611,8 @@
       <c r="P239" s="1"/>
       <c r="Q239" s="1"/>
       <c r="R239" s="1"/>
-      <c r="S239" s="1"/>
-    </row>
-    <row r="240" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -5940,9 +5631,8 @@
       <c r="P240" s="1"/>
       <c r="Q240" s="1"/>
       <c r="R240" s="1"/>
-      <c r="S240" s="1"/>
-    </row>
-    <row r="241" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -5961,9 +5651,8 @@
       <c r="P241" s="1"/>
       <c r="Q241" s="1"/>
       <c r="R241" s="1"/>
-      <c r="S241" s="1"/>
-    </row>
-    <row r="242" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -5982,9 +5671,8 @@
       <c r="P242" s="1"/>
       <c r="Q242" s="1"/>
       <c r="R242" s="1"/>
-      <c r="S242" s="1"/>
-    </row>
-    <row r="243" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -6003,9 +5691,8 @@
       <c r="P243" s="1"/>
       <c r="Q243" s="1"/>
       <c r="R243" s="1"/>
-      <c r="S243" s="1"/>
-    </row>
-    <row r="244" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -6024,9 +5711,8 @@
       <c r="P244" s="1"/>
       <c r="Q244" s="1"/>
       <c r="R244" s="1"/>
-      <c r="S244" s="1"/>
-    </row>
-    <row r="245" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -6045,9 +5731,8 @@
       <c r="P245" s="1"/>
       <c r="Q245" s="1"/>
       <c r="R245" s="1"/>
-      <c r="S245" s="1"/>
-    </row>
-    <row r="246" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -6066,9 +5751,8 @@
       <c r="P246" s="1"/>
       <c r="Q246" s="1"/>
       <c r="R246" s="1"/>
-      <c r="S246" s="1"/>
-    </row>
-    <row r="247" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -6087,9 +5771,8 @@
       <c r="P247" s="1"/>
       <c r="Q247" s="1"/>
       <c r="R247" s="1"/>
-      <c r="S247" s="1"/>
-    </row>
-    <row r="248" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -6108,9 +5791,8 @@
       <c r="P248" s="1"/>
       <c r="Q248" s="1"/>
       <c r="R248" s="1"/>
-      <c r="S248" s="1"/>
-    </row>
-    <row r="249" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -6129,9 +5811,8 @@
       <c r="P249" s="1"/>
       <c r="Q249" s="1"/>
       <c r="R249" s="1"/>
-      <c r="S249" s="1"/>
-    </row>
-    <row r="250" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
@@ -6150,9 +5831,8 @@
       <c r="P250" s="1"/>
       <c r="Q250" s="1"/>
       <c r="R250" s="1"/>
-      <c r="S250" s="1"/>
-    </row>
-    <row r="251" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -6171,9 +5851,8 @@
       <c r="P251" s="1"/>
       <c r="Q251" s="1"/>
       <c r="R251" s="1"/>
-      <c r="S251" s="1"/>
-    </row>
-    <row r="252" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
@@ -6192,9 +5871,8 @@
       <c r="P252" s="1"/>
       <c r="Q252" s="1"/>
       <c r="R252" s="1"/>
-      <c r="S252" s="1"/>
-    </row>
-    <row r="253" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -6213,9 +5891,8 @@
       <c r="P253" s="1"/>
       <c r="Q253" s="1"/>
       <c r="R253" s="1"/>
-      <c r="S253" s="1"/>
-    </row>
-    <row r="254" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
@@ -6234,9 +5911,8 @@
       <c r="P254" s="1"/>
       <c r="Q254" s="1"/>
       <c r="R254" s="1"/>
-      <c r="S254" s="1"/>
-    </row>
-    <row r="255" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" ht="14.4" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
@@ -6255,112 +5931,236 @@
       <c r="P255" s="1"/>
       <c r="Q255" s="1"/>
       <c r="R255" s="1"/>
-      <c r="S255" s="1"/>
-    </row>
-    <row r="256" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A256" s="1"/>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
-      <c r="D256" s="1"/>
-      <c r="E256" s="1"/>
-      <c r="F256" s="1"/>
-      <c r="G256" s="1"/>
-      <c r="H256" s="1"/>
-      <c r="I256" s="1"/>
-      <c r="J256" s="1"/>
-      <c r="K256" s="1"/>
-      <c r="L256" s="1"/>
-      <c r="M256" s="1"/>
-      <c r="N256" s="1"/>
-      <c r="O256" s="1"/>
-      <c r="P256" s="1"/>
-      <c r="Q256" s="1"/>
-      <c r="R256" s="1"/>
-      <c r="S256" s="1"/>
-    </row>
-    <row r="257" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A257" s="1"/>
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
-      <c r="D257" s="1"/>
-      <c r="E257" s="1"/>
-      <c r="F257" s="1"/>
-      <c r="G257" s="1"/>
-      <c r="H257" s="1"/>
-      <c r="I257" s="1"/>
-      <c r="J257" s="1"/>
-      <c r="K257" s="1"/>
-      <c r="L257" s="1"/>
-      <c r="M257" s="1"/>
-      <c r="N257" s="1"/>
-      <c r="O257" s="1"/>
-      <c r="P257" s="1"/>
-      <c r="Q257" s="1"/>
-      <c r="R257" s="1"/>
-      <c r="S257" s="1"/>
-    </row>
-    <row r="258" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A258" s="1"/>
-      <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
-      <c r="D258" s="1"/>
-      <c r="E258" s="1"/>
-      <c r="F258" s="1"/>
-      <c r="G258" s="1"/>
-      <c r="H258" s="1"/>
-      <c r="I258" s="1"/>
-      <c r="J258" s="1"/>
-      <c r="K258" s="1"/>
-      <c r="L258" s="1"/>
-      <c r="M258" s="1"/>
-      <c r="N258" s="1"/>
-      <c r="O258" s="1"/>
-      <c r="P258" s="1"/>
-      <c r="Q258" s="1"/>
-      <c r="R258" s="1"/>
-      <c r="S258" s="1"/>
-    </row>
-    <row r="259" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A259" s="1"/>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
-      <c r="D259" s="1"/>
-      <c r="E259" s="1"/>
-      <c r="F259" s="1"/>
-      <c r="G259" s="1"/>
-      <c r="H259" s="1"/>
-      <c r="I259" s="1"/>
-      <c r="J259" s="1"/>
-      <c r="K259" s="1"/>
-      <c r="L259" s="1"/>
-      <c r="M259" s="1"/>
-      <c r="N259" s="1"/>
-      <c r="O259" s="1"/>
-      <c r="P259" s="1"/>
-      <c r="Q259" s="1"/>
-      <c r="R259" s="1"/>
-      <c r="S259" s="1"/>
-    </row>
-    <row r="260" ht="14.4" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A260" s="1"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
-      <c r="E260" s="1"/>
-      <c r="F260" s="1"/>
-      <c r="G260" s="1"/>
-      <c r="H260" s="1"/>
-      <c r="I260" s="1"/>
-      <c r="J260" s="1"/>
-      <c r="K260" s="1"/>
-      <c r="L260" s="1"/>
-      <c r="M260" s="1"/>
-      <c r="N260" s="1"/>
-      <c r="O260" s="1"/>
-      <c r="P260" s="1"/>
-      <c r="Q260" s="1"/>
-      <c r="R260" s="1"/>
-      <c r="S260" s="1"/>
+    </row>
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>8</v>
+      </c>
+      <c r="C256" t="s">
+        <v>51</v>
+      </c>
+      <c r="D256" t="s">
+        <v>52</v>
+      </c>
+      <c r="E256" t="s">
+        <v>53</v>
+      </c>
+      <c r="F256" t="s">
+        <v>54</v>
+      </c>
+      <c r="G256" t="s">
+        <v>55</v>
+      </c>
+      <c r="I256" t="s">
+        <v>56</v>
+      </c>
+      <c r="J256" t="s">
+        <v>57</v>
+      </c>
+      <c r="M256" t="s">
+        <v>39</v>
+      </c>
+      <c r="N256" t="s">
+        <v>56</v>
+      </c>
+      <c r="O256" t="s">
+        <v>58</v>
+      </c>
+      <c r="P256" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q256" t="s">
+        <v>42</v>
+      </c>
+      <c r="R256" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="257" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>9</v>
+      </c>
+      <c r="C257" t="s">
+        <v>51</v>
+      </c>
+      <c r="D257" t="s">
+        <v>52</v>
+      </c>
+      <c r="E257" t="s">
+        <v>61</v>
+      </c>
+      <c r="F257" t="s">
+        <v>62</v>
+      </c>
+      <c r="G257" t="s">
+        <v>63</v>
+      </c>
+      <c r="I257" t="s">
+        <v>36</v>
+      </c>
+      <c r="J257" t="s">
+        <v>64</v>
+      </c>
+      <c r="K257" t="s">
+        <v>37</v>
+      </c>
+      <c r="M257" t="s">
+        <v>65</v>
+      </c>
+      <c r="N257" t="s">
+        <v>36</v>
+      </c>
+      <c r="O257" t="s">
+        <v>66</v>
+      </c>
+      <c r="P257" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q257" t="s">
+        <v>42</v>
+      </c>
+      <c r="R257" t="s">
+        <v>67</v>
+      </c>
+      <c r="T257" t="s">
+        <v>57</v>
+      </c>
+      <c r="U257" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y257" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC257" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="258" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>10</v>
+      </c>
+      <c r="C258" t="s">
+        <v>51</v>
+      </c>
+      <c r="D258" t="s">
+        <v>52</v>
+      </c>
+      <c r="E258" t="s">
+        <v>68</v>
+      </c>
+      <c r="F258" t="s">
+        <v>62</v>
+      </c>
+      <c r="G258" t="s">
+        <v>63</v>
+      </c>
+      <c r="I258" t="s">
+        <v>56</v>
+      </c>
+      <c r="J258" t="s">
+        <v>57</v>
+      </c>
+      <c r="K258" t="s">
+        <v>37</v>
+      </c>
+      <c r="M258" t="s">
+        <v>65</v>
+      </c>
+      <c r="N258" t="s">
+        <v>56</v>
+      </c>
+      <c r="O258" t="s">
+        <v>69</v>
+      </c>
+      <c r="P258" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q258" t="s">
+        <v>42</v>
+      </c>
+      <c r="R258" t="s">
+        <v>71</v>
+      </c>
+      <c r="T258" t="s">
+        <v>64</v>
+      </c>
+      <c r="U258" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y258" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC258" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD258" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="259" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>7</v>
+      </c>
+      <c r="C259" t="s">
+        <v>73</v>
+      </c>
+      <c r="D259" t="s">
+        <v>74</v>
+      </c>
+      <c r="E259" t="s">
+        <v>75</v>
+      </c>
+      <c r="F259" t="s">
+        <v>76</v>
+      </c>
+      <c r="G259" t="s">
+        <v>77</v>
+      </c>
+      <c r="I259" t="s">
+        <v>56</v>
+      </c>
+      <c r="J259" t="s">
+        <v>57</v>
+      </c>
+      <c r="K259" t="s">
+        <v>37</v>
+      </c>
+      <c r="M259" t="s">
+        <v>78</v>
+      </c>
+      <c r="N259" t="s">
+        <v>36</v>
+      </c>
+      <c r="O259" t="s">
+        <v>79</v>
+      </c>
+      <c r="P259" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q259" t="s">
+        <v>42</v>
+      </c>
+      <c r="R259" t="s">
+        <v>81</v>
+      </c>
+      <c r="U259" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y259" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD259" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE259" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF259" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG259" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>